<commit_message>
Bugfix: find some hex in log string fail
</commit_message>
<xml_diff>
--- a/script/charm.xlsx
+++ b/script/charm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xiayuguo/mhw_pc_armor_editor/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7146DE-EF9D-DE4C-A8C1-8D998B79948F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4EEAED-BD15-994C-89C7-A50C110F9989}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="2740" windowWidth="25840" windowHeight="14440" xr2:uid="{AF8F22B8-E06C-064E-B168-BC8F456CDDE4}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="580">
   <si>
     <t>技能id</t>
   </si>
@@ -1722,15 +1722,87 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>注：技能和技能等级可以留空，其中技能3留空则保留原有技能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>解放护石3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>耳塞护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>达人护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>匠护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>友爱护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>挑战护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>铁壁护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>昂扬护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>利刃护石</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>麻痹护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>睡眠护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆破护石4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>火护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>水护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冰护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龙护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>毒护石5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>集中护石3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>体力护石3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>注：技能和技能等级可以留空，其中技能3留空则保留原有技能</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2131,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9FD5401-EBD4-F440-90F9-87E04DA63BEA}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2144,7 +2216,7 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="3" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2202,84 +2274,822 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>292</v>
       </c>
       <c r="G3">
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="I3">
         <v>3</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>453</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="M3">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4" t="s">
+        <v>164</v>
+      </c>
+      <c r="K4">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4">
+      <c r="L4" t="s">
+        <v>227</v>
+      </c>
+      <c r="M4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>562</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
         <v>3</v>
       </c>
-      <c r="F4" t="s">
-        <v>451</v>
-      </c>
-      <c r="G4">
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K5">
         <v>3</v>
       </c>
-      <c r="H4" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4">
+      <c r="L5" t="s">
+        <v>227</v>
+      </c>
+      <c r="M5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>563</v>
+      </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6">
         <v>3</v>
       </c>
-      <c r="J4" t="s">
-        <v>188</v>
-      </c>
-      <c r="K4">
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6" t="s">
+        <v>179</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>227</v>
+      </c>
+      <c r="M6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>573</v>
+      </c>
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>87</v>
+      </c>
+      <c r="I7">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>182</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>227</v>
+      </c>
+      <c r="M7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>574</v>
+      </c>
+      <c r="B8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>90</v>
+      </c>
+      <c r="I8">
+        <v>5</v>
+      </c>
+      <c r="J8" t="s">
+        <v>182</v>
+      </c>
+      <c r="K8">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>227</v>
+      </c>
+      <c r="M8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>575</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>182</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9" t="s">
+        <v>227</v>
+      </c>
+      <c r="M9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>576</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>96</v>
+      </c>
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10" t="s">
+        <v>182</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10" t="s">
+        <v>227</v>
+      </c>
+      <c r="M10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>577</v>
+      </c>
+      <c r="B11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>182</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>227</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>578</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>461</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>167</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12">
+        <v>4</v>
+      </c>
+      <c r="J12" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12">
+        <v>3</v>
+      </c>
+      <c r="L12" t="s">
+        <v>227</v>
+      </c>
+      <c r="M12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>570</v>
+      </c>
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>461</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13" t="s">
+        <v>105</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13" t="s">
+        <v>227</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>571</v>
+      </c>
+      <c r="B14" t="s">
+        <v>108</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>461</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14" t="s">
+        <v>167</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I14">
+        <v>4</v>
+      </c>
+      <c r="J14" t="s">
+        <v>54</v>
+      </c>
+      <c r="K14">
+        <v>3</v>
+      </c>
+      <c r="L14" t="s">
+        <v>227</v>
+      </c>
+      <c r="M14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>572</v>
+      </c>
+      <c r="B15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>461</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15" t="s">
+        <v>167</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15" t="s">
+        <v>111</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15">
+        <v>3</v>
+      </c>
+      <c r="L15" t="s">
+        <v>227</v>
+      </c>
+      <c r="M15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>569</v>
+      </c>
+      <c r="B16" t="s">
+        <v>432</v>
+      </c>
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="L4" t="s">
-        <v>139</v>
-      </c>
-      <c r="M4">
-        <v>7</v>
+      <c r="D16" t="s">
+        <v>292</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>414</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>453</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>161</v>
+      </c>
+      <c r="K16">
+        <v>3</v>
+      </c>
+      <c r="L16" t="s">
+        <v>182</v>
+      </c>
+      <c r="M16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" t="s">
+        <v>568</v>
+      </c>
+      <c r="B17" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E17">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>230</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+      <c r="H17" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17" t="s">
+        <v>345</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+      <c r="L17" t="s">
+        <v>149</v>
+      </c>
+      <c r="M17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" t="s">
+        <v>567</v>
+      </c>
+      <c r="B18" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>233</v>
+      </c>
+      <c r="I18">
+        <v>5</v>
+      </c>
+      <c r="J18" t="s">
+        <v>482</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+      <c r="L18" t="s">
+        <v>182</v>
+      </c>
+      <c r="M18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" t="s">
+        <v>566</v>
+      </c>
+      <c r="B19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C19">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>179</v>
+      </c>
+      <c r="I19">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
+        <v>280</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19" t="s">
+        <v>227</v>
+      </c>
+      <c r="M19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" t="s">
+        <v>565</v>
+      </c>
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>511</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>242</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20" t="s">
+        <v>239</v>
+      </c>
+      <c r="I20">
+        <v>5</v>
+      </c>
+      <c r="J20" t="s">
+        <v>345</v>
+      </c>
+      <c r="K20">
+        <v>3</v>
+      </c>
+      <c r="L20" t="s">
+        <v>280</v>
+      </c>
+      <c r="M20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" t="s">
+        <v>564</v>
+      </c>
+      <c r="B21" t="s">
+        <v>155</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>57</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21" t="s">
+        <v>155</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21" t="s">
+        <v>182</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21" t="s">
+        <v>227</v>
+      </c>
+      <c r="M21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" t="s">
+        <v>579</v>
+      </c>
+      <c r="B22" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22" t="s">
+        <v>149</v>
+      </c>
+      <c r="I22">
+        <v>3</v>
+      </c>
+      <c r="J22" t="s">
+        <v>191</v>
+      </c>
+      <c r="K22">
+        <v>5</v>
+      </c>
+      <c r="L22" t="s">
+        <v>227</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2288,7 +3098,7 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{830BA88A-793D-BE46-8D8C-C18107A57F56}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I15 I17:I22 C2:C1048576" xr:uid="{830BA88A-793D-BE46-8D8C-C18107A57F56}">
       <formula1>0</formula1>
       <formula2>7</formula2>
     </dataValidation>
@@ -2301,7 +3111,7 @@
           <x14:formula1>
             <xm:f>skill!$C$2:$C$218</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B1048576 F2:F1048576 D2:D1048576 H2:H1048576 J2:J1048576 L2:L1048576</xm:sqref>
+          <xm:sqref>J2:J1048576 F2:F1048576 H2:H1048576 B2:B1048576 D2:D1048576 L2:L1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2313,8 +3123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9037A566-145D-F448-9363-EBEFF76415C6}">
   <dimension ref="A1:E218"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E201" sqref="E201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>